<commit_message>
Import Data Allocation Validation
validation for imported spreadsheet to ensure all unallocated units are presented as a warning
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jacob\University\IFB398 - Capstone Phase 1\TeacherAllocationSystem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43AA34A-1032-4EF0-A516-EF39D9EB2D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="7650" yWindow="1260" windowWidth="21240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -680,7 +689,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -886,8 +895,8 @@
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -1150,7 +1159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1183,9 +1192,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1218,6 +1244,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1393,14 +1436,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CO59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="BQ30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="AA21" sqref="AA21"/>
+      <selection pane="bottomRight" activeCell="CF32" sqref="CF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,7 +3418,7 @@
       </c>
       <c r="CF7" s="23">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG7" s="1"/>
       <c r="CH7" s="1"/>
@@ -3722,7 +3765,7 @@
       </c>
       <c r="CF8" s="23">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CG8" s="1"/>
       <c r="CH8" s="1"/>
@@ -6715,11 +6758,11 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="11"/>
-        <v>2.2156766477455796</v>
+        <v>1.1742839625873545</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="9"/>
-        <v>-0.32196166825827177</v>
+        <v>-1.3633543534164969</v>
       </c>
       <c r="BU47" s="31">
         <v>0.2</v>
@@ -6727,9 +6770,7 @@
       <c r="CB47" s="2">
         <v>1</v>
       </c>
-      <c r="CF47" s="37">
-        <v>1</v>
-      </c>
+      <c r="CF47" s="37"/>
     </row>
     <row r="48" spans="1:91" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -7329,7 +7370,7 @@
       <c r="BU59" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A9:CO48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:CO48">
     <sortCondition descending="1" ref="G9:G48"/>
   </sortState>
   <conditionalFormatting sqref="AB8:AC8 AF8 BG8:BW8 CA8:CD8 Y8 AH8:BD8 CM8:CN8 H8:T8">
@@ -7578,7 +7619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7609,7 +7650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'dev' of https://github.com/JessWill/TeacherAllocationSystem into dev"
This reverts commit b7b2290e33f24c8562e25cf70d94513328f21d32, reversing
changes made to ed9f5a89d9706232a54a7bb48caccce7719d4a8f.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,31 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jacob\University\IFB398 - Capstone Phase 1\TeacherAllocationSystem\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43AA34A-1032-4EF0-A516-EF39D9EB2D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="1260" windowWidth="21240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -689,7 +680,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -895,8 +886,8 @@
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="2"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -1159,7 +1150,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1192,26 +1183,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1244,23 +1218,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1436,14 +1393,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CO59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="BQ30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="CF32" sqref="CF32"/>
+      <selection pane="bottomRight" activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,7 +3375,7 @@
       </c>
       <c r="CF7" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG7" s="1"/>
       <c r="CH7" s="1"/>
@@ -3765,7 +3722,7 @@
       </c>
       <c r="CF8" s="23">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CG8" s="1"/>
       <c r="CH8" s="1"/>
@@ -6758,11 +6715,11 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="11"/>
-        <v>1.1742839625873545</v>
+        <v>2.2156766477455796</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="9"/>
-        <v>-1.3633543534164969</v>
+        <v>-0.32196166825827177</v>
       </c>
       <c r="BU47" s="31">
         <v>0.2</v>
@@ -6770,7 +6727,9 @@
       <c r="CB47" s="2">
         <v>1</v>
       </c>
-      <c r="CF47" s="37"/>
+      <c r="CF47" s="37">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:91" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -7370,7 +7329,7 @@
       <c r="BU59" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:CO48">
+  <sortState ref="A9:CO48">
     <sortCondition descending="1" ref="G9:G48"/>
   </sortState>
   <conditionalFormatting sqref="AB8:AC8 AF8 BG8:BW8 CA8:CD8 Y8 AH8:BD8 CM8:CN8 H8:T8">
@@ -7619,7 +7578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7650,7 +7609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'dev' of https://github.com/JessWill/TeacherAllocationSystem into dev""
This reverts commit 9006a04deaa101aaf73927807756f76960e0b97e.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jacob\University\IFB398 - Capstone Phase 1\TeacherAllocationSystem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43AA34A-1032-4EF0-A516-EF39D9EB2D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="7650" yWindow="1260" windowWidth="21240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -680,7 +689,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -886,8 +895,8 @@
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -1150,7 +1159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1183,9 +1192,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1218,6 +1244,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1393,14 +1436,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CO59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="BQ30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="AA21" sqref="AA21"/>
+      <selection pane="bottomRight" activeCell="CF32" sqref="CF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,7 +3418,7 @@
       </c>
       <c r="CF7" s="23">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG7" s="1"/>
       <c r="CH7" s="1"/>
@@ -3722,7 +3765,7 @@
       </c>
       <c r="CF8" s="23">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CG8" s="1"/>
       <c r="CH8" s="1"/>
@@ -6715,11 +6758,11 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="11"/>
-        <v>2.2156766477455796</v>
+        <v>1.1742839625873545</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="9"/>
-        <v>-0.32196166825827177</v>
+        <v>-1.3633543534164969</v>
       </c>
       <c r="BU47" s="31">
         <v>0.2</v>
@@ -6727,9 +6770,7 @@
       <c r="CB47" s="2">
         <v>1</v>
       </c>
-      <c r="CF47" s="37">
-        <v>1</v>
-      </c>
+      <c r="CF47" s="37"/>
     </row>
     <row r="48" spans="1:91" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -7329,7 +7370,7 @@
       <c r="BU59" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A9:CO48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:CO48">
     <sortCondition descending="1" ref="G9:G48"/>
   </sortState>
   <conditionalFormatting sqref="AB8:AC8 AF8 BG8:BW8 CA8:CD8 Y8 AH8:BD8 CM8:CN8 H8:T8">
@@ -7578,7 +7619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7609,7 +7650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
export functionality completed and student and share info imported and stored in DB
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jacob\University\IFB398 - Capstone Phase 1\TeacherAllocationSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43AA34A-1032-4EF0-A516-EF39D9EB2D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28300F7-67CB-40EE-A7E9-7B6519B200B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="1260" windowWidth="21240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27105" yWindow="1890" windowWidth="21240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation" sheetId="1" r:id="rId1"/>
@@ -1440,10 +1440,10 @@
   <dimension ref="A1:CO59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="BQ30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="AU30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="CF32" sqref="CF32"/>
+      <selection pane="bottomRight" activeCell="BE41" sqref="BE41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,6 +2969,7 @@
         <v>0.5</v>
       </c>
       <c r="BE6" s="11">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="BF6" s="11">
@@ -7662,6 +7663,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005144375E58E94B4797547602088A153E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e63007d8e5e8654fe70b8510975bcc0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d0ad2d52-4869-465d-a93a-001fa21a593d" xmlns:ns4="a21de7b9-cad9-43f2-8459-9b1b4f9894e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c71fdf4a3f812f4c6f43eee57994d278" ns3:_="" ns4:_="">
     <xsd:import namespace="d0ad2d52-4869-465d-a93a-001fa21a593d"/>
@@ -7884,36 +7900,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26B64111-6351-4AC4-ABBC-45415AA1E95B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E6D528A-3708-4901-8018-58179A887951}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d0ad2d52-4869-465d-a93a-001fa21a593d"/>
-    <ds:schemaRef ds:uri="a21de7b9-cad9-43f2-8459-9b1b4f9894e2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7936,9 +7926,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E6D528A-3708-4901-8018-58179A887951}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26B64111-6351-4AC4-ABBC-45415AA1E95B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d0ad2d52-4869-465d-a93a-001fa21a593d"/>
+    <ds:schemaRef ds:uri="a21de7b9-cad9-43f2-8459-9b1b4f9894e2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>